<commit_message>
gen gabors to test range model confidence
</commit_message>
<xml_diff>
--- a/projects/1-CNN/results.xlsx
+++ b/projects/1-CNN/results.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan\Documents\GitHub\neuralnets\projects\1-CNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0B441D0-CC6C-436A-AA38-AEEF75358314}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436F6E9E-8E89-4E54-B443-88D5159EC894}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25800" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{382EE61A-D709-4356-8919-042026195128}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="1110" activeTab="1" xr2:uid="{382EE61A-D709-4356-8919-042026195128}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Model 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Model 2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Tilt</t>
   </si>
@@ -43,9 +44,6 @@
   </si>
   <si>
     <t>Model: Conv base w classifier at last layer</t>
-  </si>
-  <si>
-    <t>Trained on: 20,000 images with tilt 2.26 + contrast 1</t>
   </si>
   <si>
     <t>High Conf: 0.36
@@ -148,13 +146,33 @@
   </si>
   <si>
     <t>The model appears biased towards the tilt + contrast it was trained on. Highest conf in 2.26 avg and 1 contrast</t>
+  </si>
+  <si>
+    <t>High Conf: 0.38
+Tf Acc: 0.61
+My Acc: 0.66</t>
+  </si>
+  <si>
+    <t>tilts</t>
+  </si>
+  <si>
+    <t>contrasts 0.3, 0.45, 1</t>
+  </si>
+  <si>
+    <t>Range model</t>
+  </si>
+  <si>
+    <t>Trained on: 20,000 images with tilt 2.26 + contrast 1, threshold = 2</t>
+  </si>
+  <si>
+    <t>Trained on: 18,000 images with tilts [0.1, 0.2, 0.4, 0.8, 1.6, 3.2] &amp; contrasts [0.3, 0.45, 1], threshold = 0.5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +183,14 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -191,15 +217,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -208,6 +228,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -524,8 +551,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3564C984-96C4-4BC7-9CD1-1591A1E566AE}">
   <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,15 +568,15 @@
     </row>
     <row r="3" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
@@ -562,92 +589,92 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" s="4" t="s">
+    <row r="7" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="4"/>
+      <c r="C7" s="3">
+        <v>2.2599999999999998</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4"/>
+      <c r="C8" s="3">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="5">
-        <v>2.2599999999999998</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="4" t="s">
+      <c r="G8" s="2" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="5">
-        <v>4.5199999999999996</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="F9" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C12" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="2:7" x14ac:dyDescent="0.25">
       <c r="C13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -658,4 +685,76 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA12FB55-1A2B-44DB-8E20-09BF3B45978C}">
+  <dimension ref="B2:C13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C2" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>1.6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>3.2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update results and simulation for testing
</commit_message>
<xml_diff>
--- a/projects/1-CNN/results.xlsx
+++ b/projects/1-CNN/results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryan\Documents\GitHub\neuralnets\projects\1-CNN\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436F6E9E-8E89-4E54-B443-88D5159EC894}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{181D2D9B-079A-4FCD-85AF-2BBBAF614D14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11280" windowHeight="1110" activeTab="1" xr2:uid="{382EE61A-D709-4356-8919-042026195128}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{382EE61A-D709-4356-8919-042026195128}"/>
   </bookViews>
   <sheets>
     <sheet name="Model 1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Tilt</t>
   </si>
@@ -166,6 +166,54 @@
   </si>
   <si>
     <t>Trained on: 18,000 images with tilts [0.1, 0.2, 0.4, 0.8, 1.6, 3.2] &amp; contrasts [0.3, 0.45, 1], threshold = 0.5</t>
+  </si>
+  <si>
+    <t>High Conf: 0.33
+Tf Acc: 0.52
+My Acc: 0.55</t>
+  </si>
+  <si>
+    <t>High Conf: 0.35
+Tf Acc: 0.56
+My Acc: 0.61</t>
+  </si>
+  <si>
+    <t>High Conf: 0.36
+Tf Acc: 0.61
+My Acc: 0.67</t>
+  </si>
+  <si>
+    <t>High Conf: 0.43
+Tf Acc: 0.68
+My Acc: 0.75</t>
+  </si>
+  <si>
+    <t>High Conf: 0.48
+Tf Acc: 0.72
+My Acc: 0.82</t>
+  </si>
+  <si>
+    <t>High Conf: 0.33
+Tf Acc: 0.53
+My Acc: 0.56</t>
+  </si>
+  <si>
+    <t>Observations</t>
+  </si>
+  <si>
+    <t>The High Conf (0.38) and My Acc (0.66) calculated using the test set comprised of the full range of tilts and contrasts reflected an average of all the High Conf and My Acc calculations across tilts</t>
+  </si>
+  <si>
+    <t>The confidence began slowly ticking up at the third tilt (0.4) and took a large jump in the fifth tilt (1.6)</t>
+  </si>
+  <si>
+    <t>The first two tilts (0.1 &amp; 0.2) were too slight for the model to discriminate between very well.</t>
+  </si>
+  <si>
+    <t>Not until the 4th tilt (0.8) was there a more noticeable performance above chance (0.6+)</t>
+  </si>
+  <si>
+    <t>The model becomes more confident and performs better as the tilts become greater</t>
   </si>
 </sst>
 </file>
@@ -217,7 +265,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -228,13 +276,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,11 +624,11 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="D5" s="1">
@@ -593,7 +645,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>0</v>
       </c>
       <c r="C6" s="3">
@@ -613,7 +665,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="4"/>
+      <c r="B7" s="5"/>
       <c r="C7" s="3">
         <v>2.2599999999999998</v>
       </c>
@@ -631,7 +683,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="4"/>
+      <c r="B8" s="5"/>
       <c r="C8" s="3">
         <v>4.5199999999999996</v>
       </c>
@@ -689,10 +741,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA12FB55-1A2B-44DB-8E20-09BF3B45978C}">
-  <dimension ref="B2:C13"/>
+  <dimension ref="B2:D20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -700,57 +752,103 @@
     <col min="3" max="3" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C2" s="6" t="s">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="2:3" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B7" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="4" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>0.8</v>
       </c>
-    </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>1.6</v>
       </c>
-    </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="2:4" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>3.2</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D20" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>